<commit_message>
Updated final PDFs. Added reverse strand antisense microhomologies.
</commit_message>
<xml_diff>
--- a/Antisense_MH_list.xlsx
+++ b/Antisense_MH_list.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngkyu/Desktop/Bio_info/Data/Penghao_analysis/antisense_output_20220606/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5653B201-D0CA-4C47-B9EB-C9CF253585BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC27980-D9A8-214E-AC47-3A9DBD3504DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="3300" windowWidth="26840" windowHeight="15940" xr2:uid="{37A2D933-8318-1646-ADB3-D9A8FB200410}"/>
+    <workbookView xWindow="6560" yWindow="2580" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{37A2D933-8318-1646-ADB3-D9A8FB200410}"/>
   </bookViews>
   <sheets>
-    <sheet name="All_microhomology" sheetId="1" r:id="rId1"/>
+    <sheet name="Forward" sheetId="1" r:id="rId1"/>
+    <sheet name="Reverse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -221,6 +222,150 @@
   </si>
   <si>
     <t>TGATGAACTTCGAGGACGGCGGCGTGGCGACCGTGACCCAGGACGGCTGCTTCATCTACAAGGTGAAGTTCATCGGCGTGAACTTCC</t>
+  </si>
+  <si>
+    <t>EE1R</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>CCT</t>
+  </si>
+  <si>
+    <t>ATGAACTTCACCTCGAAGTTCAT</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE2R</t>
+  </si>
+  <si>
+    <t>GCCGTCC</t>
+  </si>
+  <si>
+    <t>AGATGAAGCAGCCGTCCTCGAAGTTCA</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTTGTAGATGAAGCAGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE3R</t>
+  </si>
+  <si>
+    <t>GCCG</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGTCCTCGAAGT</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE4R</t>
+  </si>
+  <si>
+    <t>AGATGAAGCAGCCGCCGTCCTCGA</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTTGTAGATGAAGCAGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE5R</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGCCGTCCTCGA</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE6R</t>
+  </si>
+  <si>
+    <t>CAC</t>
+  </si>
+  <si>
+    <t>CGATGAACTTCACGCCGCCGTCC</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE7R</t>
+  </si>
+  <si>
+    <t>GCC</t>
+  </si>
+  <si>
+    <t>AGATGAAGCAGCCACGCCGCCGT</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTTGTAGATGAAGCAGCCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE8R</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCACGCCGCCGT</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE9R</t>
+  </si>
+  <si>
+    <t>GTC</t>
+  </si>
+  <si>
+    <t>TGAAGCAGCCGTCGCCACGCCGC</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTTGTAGATGAAGCAGCCGTCGCCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE10R</t>
+  </si>
+  <si>
+    <t>TCAC</t>
+  </si>
+  <si>
+    <t>CCGATGAACTTCACGGTCGCCACG</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACGGTCGCCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE11R</t>
+  </si>
+  <si>
+    <t>TGAAGCAGCCGTCACGGTCGCCA</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTTGTAGATGAAGCAGCCGTCACGGTCGCCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE12R</t>
+  </si>
+  <si>
+    <t>ATGAACTTCACCTGGGTCACGGT</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTGGGTCACGGTCGCCACGCCGCCGTCCTCGAAGTTCATCA</t>
+  </si>
+  <si>
+    <t>EE13R</t>
+  </si>
+  <si>
+    <t>GTCC</t>
+  </si>
+  <si>
+    <t>TGAAGCAGCCGTCCTGGGTCACGG</t>
+  </si>
+  <si>
+    <t>GGAAGTTCACGCCGATGAACTTCACCTTGTAGATGAAGCAGCCGTCCTGGGTCACGGTCGCCACGCCGCCGTCCTCGAAGTTCATCA</t>
   </si>
 </sst>
 </file>
@@ -609,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAC2E73-C045-234B-BB49-0A4C60DA2463}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -1482,4 +1627,883 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DD1D77-F484-B742-AF4E-680786BEC78D}">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1">
+        <v>223</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1">
+        <v>217</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4">
+        <v>41</v>
+      </c>
+      <c r="G4">
+        <v>218</v>
+      </c>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>212</v>
+      </c>
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2">
+        <v>218</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="2">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2">
+        <v>212</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2">
+        <v>215</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="2">
+        <v>41</v>
+      </c>
+      <c r="G9" s="2">
+        <v>209</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2">
+        <v>215</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="2">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2">
+        <v>209</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>212</v>
+      </c>
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>206</v>
+      </c>
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="3">
+        <v>41</v>
+      </c>
+      <c r="G14" s="3">
+        <v>210</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="3">
+        <v>41</v>
+      </c>
+      <c r="G15" s="3">
+        <v>204</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="3">
+        <v>11</v>
+      </c>
+      <c r="G16" s="3">
+        <v>210</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="3">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3">
+        <v>204</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="4">
+        <v>44</v>
+      </c>
+      <c r="G18" s="4">
+        <v>207</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="4">
+        <v>44</v>
+      </c>
+      <c r="G19" s="4">
+        <v>201</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20">
+        <v>22</v>
+      </c>
+      <c r="G20">
+        <v>202</v>
+      </c>
+      <c r="H20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <v>196</v>
+      </c>
+      <c r="H21" t="s">
+        <v>97</v>
+      </c>
+      <c r="I21" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="4">
+        <v>44</v>
+      </c>
+      <c r="G22" s="4">
+        <v>201</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="4">
+        <v>44</v>
+      </c>
+      <c r="G23" s="4">
+        <v>195</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="1">
+        <v>25</v>
+      </c>
+      <c r="G24" s="1">
+        <v>196</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="1">
+        <v>25</v>
+      </c>
+      <c r="G25" s="1">
+        <v>190</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26">
+        <v>44</v>
+      </c>
+      <c r="G26">
+        <v>194</v>
+      </c>
+      <c r="H26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27">
+        <v>44</v>
+      </c>
+      <c r="G27">
+        <v>188</v>
+      </c>
+      <c r="H27" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" t="s">
+        <v>108</v>
+      </c>
+      <c r="J27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the microhomology lists.
</commit_message>
<xml_diff>
--- a/Antisense_MH_list.xlsx
+++ b/Antisense_MH_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngkyu/Desktop/Bio_info/Data/Penghao_analysis/antisense_output_20220606/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC27980-D9A8-214E-AC47-3A9DBD3504DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADD8A58-7099-BE43-9A5F-05E0AC8E5310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="2580" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{37A2D933-8318-1646-ADB3-D9A8FB200410}"/>
+    <workbookView xWindow="39940" yWindow="900" windowWidth="26840" windowHeight="15940" xr2:uid="{37A2D933-8318-1646-ADB3-D9A8FB200410}"/>
   </bookViews>
   <sheets>
     <sheet name="Forward" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,25 +397,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC7F4A3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA3EFF4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD0A3F4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4A8A3"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,10 +416,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,169 +736,169 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAC2E73-C045-234B-BB49-0A4C60DA2463}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2">
         <v>211</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2">
         <v>205</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>14</v>
-      </c>
-      <c r="G4">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3">
         <v>191</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5">
-        <v>14</v>
-      </c>
-      <c r="G5">
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3">
         <v>185</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -984,327 +966,327 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4">
         <v>20</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>194</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4">
         <v>20</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="4">
         <v>188</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4">
         <v>20</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="4">
         <v>224</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="4">
         <v>20</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="4">
         <v>218</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12">
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3">
         <v>24</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>213</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13">
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="3">
         <v>24</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>207</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4">
         <v>26</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="4">
         <v>195</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="4">
         <v>26</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="4">
         <v>189</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2">
         <v>26</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>225</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="2">
         <v>26</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>219</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>44</v>
       </c>
@@ -1336,7 +1318,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
@@ -1368,71 +1350,71 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20">
+      <c r="B20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="3">
         <v>33</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>213</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21">
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3">
         <v>33</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>207</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>52</v>
       </c>
@@ -1464,7 +1446,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
@@ -1496,131 +1478,131 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="4">
         <v>40</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="4">
         <v>211</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="B25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="4">
         <v>40</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="4">
         <v>205</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26">
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="3">
         <v>41</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>191</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27">
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="3">
         <v>41</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>185</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1633,169 +1615,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DD1D77-F484-B742-AF4E-680786BEC78D}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="2">
         <v>25</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>223</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="2">
         <v>25</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>217</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="3">
         <v>41</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>218</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5">
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="3">
         <v>41</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>212</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1863,327 +1848,327 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="4">
         <v>41</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>215</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="4">
         <v>41</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="4">
         <v>209</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="2">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="4">
+        <v>11</v>
+      </c>
+      <c r="G10" s="4">
         <v>215</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="2">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="4">
+        <v>11</v>
+      </c>
+      <c r="G11" s="4">
         <v>209</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12">
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="3">
         <v>23</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>212</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13">
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="3">
         <v>23</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>206</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="4">
         <v>41</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="4">
         <v>210</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="4">
         <v>41</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="4">
         <v>204</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="3">
-        <v>11</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2">
         <v>210</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="3">
-        <v>11</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="2">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2">
         <v>204</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>92</v>
       </c>
@@ -2215,7 +2200,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>92</v>
       </c>
@@ -2247,71 +2232,71 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20">
+      <c r="B20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="3">
         <v>22</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>202</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21">
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="3">
         <v>22</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>196</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>100</v>
       </c>
@@ -2343,7 +2328,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>100</v>
       </c>
@@ -2375,131 +2360,131 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="4">
         <v>25</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="4">
         <v>196</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="B25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="4">
         <v>25</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="4">
         <v>190</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26">
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="3">
         <v>44</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>194</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27">
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="3">
         <v>44</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <v>188</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="3" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>